<commit_message>
Still Tuning System for different IE Ratios and Resp Rates
</commit_message>
<xml_diff>
--- a/docs/InhaleExhaleTimes.xlsx
+++ b/docs/InhaleExhaleTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\EVent-ir\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E6ADE65-046C-4598-98A4-95C40C36AC50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF70855-4918-4270-8A8A-81A012B8188F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB4A7457-6CE3-4D9D-AF09-1C004BC008C7}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,97 +432,97 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>60/(D2*(E2+1))</f>
-        <v>1.1111111111111112</v>
+        <v>3.75</v>
       </c>
       <c r="B2">
         <f>A2*E2</f>
-        <v>1.1111111111111112</v>
+        <v>3.75</v>
       </c>
       <c r="C2">
         <f>A2+B2</f>
-        <v>2.2222222222222223</v>
+        <v>7.5</v>
       </c>
       <c r="D2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="G2">
         <f>C2-A2-0.1-0.8</f>
-        <v>0.21111111111111103</v>
+        <v>2.8499999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>60/(D3*(E3+1))</f>
-        <v>0.7407407407407407</v>
+        <v>2.5</v>
       </c>
       <c r="B3">
         <f>A3*E3</f>
-        <v>1.4814814814814814</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <f>A3+B3</f>
-        <v>2.2222222222222223</v>
+        <v>7.5</v>
       </c>
       <c r="D3">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G5" si="0">C3-A3-0.1-0.8</f>
-        <v>0.58148148148148149</v>
+        <v>4.1000000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>60/(D4*(E4+1))</f>
-        <v>0.55555555555555558</v>
+        <v>1.875</v>
       </c>
       <c r="B4">
         <f>A4*E4</f>
-        <v>1.6666666666666667</v>
+        <v>5.625</v>
       </c>
       <c r="C4">
         <f>A4+B4</f>
-        <v>2.2222222222222223</v>
+        <v>7.5</v>
       </c>
       <c r="D4">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0.76666666666666661</v>
+        <v>4.7250000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>60/(D5*(E5+1))</f>
-        <v>0.44444444444444442</v>
+        <v>1.5</v>
       </c>
       <c r="B5">
         <f>A5*E5</f>
-        <v>1.7777777777777777</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f>A5+B5</f>
-        <v>2.2222222222222223</v>
+        <v>7.5</v>
       </c>
       <c r="D5">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0.87777777777777777</v>
+        <v>5.1000000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>